<commit_message>
Add protected xlsx docs
</commit_message>
<xml_diff>
--- a/front/src/assets/SOLICITAR_AHORRO_NOMINA.xlsx
+++ b/front/src/assets/SOLICITAR_AHORRO_NOMINA.xlsx
@@ -8,6 +8,9 @@
   <sheets>
     <sheet name="Table 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0" hidden="0">'Table 1'!$A$1:$I$42</definedName>
+  </definedNames>
   <calcPr/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
@@ -131,28 +134,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="10.000000"/>
       <color theme="1" tint="0.049989318521683403"/>
       <name val="Times New Roman"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.000000"/>
-      <color indexed="64"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -197,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="26">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -422,7 +417,7 @@
     <border>
       <left style="none"/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="none"/>
       <bottom style="none"/>
@@ -430,22 +425,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="none"/>
@@ -474,7 +454,7 @@
       <right style="none"/>
       <top style="none"/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -483,7 +463,7 @@
       <right style="none"/>
       <top style="none"/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -493,10 +473,10 @@
       </left>
       <right style="none"/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -504,10 +484,10 @@
       <left style="none"/>
       <right style="none"/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -517,7 +497,7 @@
       </left>
       <right style="none"/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="none"/>
       <diagonal style="none"/>
@@ -528,7 +508,7 @@
       </left>
       <right style="none"/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color auto="1"/>
@@ -604,13 +584,13 @@
     <xf fontId="2" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="5" fillId="2" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="2" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="13" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -619,19 +599,19 @@
     <xf fontId="0" fillId="2" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="4" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf fontId="5" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="5" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="5" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="6" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="6" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -646,88 +626,88 @@
     <xf fontId="0" fillId="2" borderId="17" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="18" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="2" borderId="19" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="2" borderId="18" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="4" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="6" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="6" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="3" borderId="20" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="6" fillId="3" borderId="19" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="3" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="6" fillId="3" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="2" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="2" borderId="20" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="2" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="2" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="22" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="21" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="4" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="3" wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="7" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="7" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="2" borderId="23" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="2" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="2" borderId="24" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="2" borderId="23" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="2" borderId="25" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="2" borderId="24" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="4" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="2" borderId="26" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="6" fillId="2" borderId="25" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="2" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="7" fillId="2" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="7" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3800,7 +3780,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>215804</xdr:colOff>
+      <xdr:colOff>215803</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>98283</xdr:rowOff>
     </xdr:to>
@@ -4361,7 +4341,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="100" workbookViewId="0">
       <selection activeCell="R12" activeCellId="0" sqref="R12"/>
     </sheetView>
   </sheetViews>
@@ -4792,6 +4772,9 @@
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="80" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="10" man="1" max="1048575"/>
+  </colBreaks>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>